<commit_message>
functions for plotting error and ROC curve
</commit_message>
<xml_diff>
--- a/files/results_for_the_report.xlsx
+++ b/files/results_for_the_report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krzys\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krzys\Desktop\ML repo\MLaPR\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4117B5AF-57E5-4FA6-A725-AD454E8E1E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3DF426-511E-420D-A732-BE2A3B89AA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9612" yWindow="4752" windowWidth="17280" windowHeight="8964" xr2:uid="{C99E41AA-753D-4BF4-8020-A2085D88D95B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C99E41AA-753D-4BF4-8020-A2085D88D95B}"/>
   </bookViews>
   <sheets>
     <sheet name="MVG Classifiers" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="124">
   <si>
     <t>MVG Classifiers - min DCF</t>
   </si>
@@ -474,6 +474,9 @@
   </si>
   <si>
     <t>0.910</t>
+  </si>
+  <si>
+    <t>USING PCA IN DCF PLOTS DOESN'T VISIBLY AFFECT THE PLOT</t>
   </si>
 </sst>
 </file>
@@ -850,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C0024B2-0F2E-4A19-B04A-D3E49F7063A9}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1269,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394DBA5B-867B-44BD-9736-635E4E515502}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1283,14 +1286,15 @@
     <col min="7" max="7" width="10.44140625" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" customWidth="1"/>
     <col min="9" max="9" width="8.33203125" customWidth="1"/>
+    <col min="12" max="12" width="51.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1302,7 +1306,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1322,7 +1326,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>75</v>
       </c>
@@ -1334,7 +1338,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1360,7 +1364,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -1386,7 +1390,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -1412,7 +1416,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>34</v>
       </c>
@@ -1423,8 +1427,11 @@
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -1450,7 +1457,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -1476,7 +1483,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -1502,7 +1509,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>66</v>
       </c>
@@ -1514,7 +1521,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
plots added for all logreg and mvg functions
</commit_message>
<xml_diff>
--- a/files/results_for_the_report.xlsx
+++ b/files/results_for_the_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krzys\Desktop\ML repo\MLaPR\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3DF426-511E-420D-A732-BE2A3B89AA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6826435F-C3AC-44F4-8E9E-3250E8638706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C99E41AA-753D-4BF4-8020-A2085D88D95B}"/>
   </bookViews>
@@ -854,7 +854,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1275,7 +1275,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
modifying gmm classifiers, adding plots
</commit_message>
<xml_diff>
--- a/files/results_for_the_report.xlsx
+++ b/files/results_for_the_report.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krzys\Desktop\ML repo\MLaPR\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93426044-30FE-4FBE-846C-F30A1374F276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478200BB-5E7F-42A5-B2FA-044732A4F1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C99E41AA-753D-4BF4-8020-A2085D88D95B}"/>
+    <workbookView xWindow="-10116" yWindow="3216" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{C99E41AA-753D-4BF4-8020-A2085D88D95B}"/>
   </bookViews>
   <sheets>
     <sheet name="MVG Classifiers" sheetId="1" r:id="rId1"/>
     <sheet name="Logistic Reg" sheetId="2" r:id="rId2"/>
     <sheet name="SVM" sheetId="3" r:id="rId3"/>
+    <sheet name="GMM" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="233">
   <si>
     <t>MVG Classifiers - min DCF</t>
   </si>
@@ -550,11 +551,293 @@
       <t xml:space="preserve"> = 0.01)</t>
     </r>
   </si>
+  <si>
+    <t>GMM -  minDCF</t>
+  </si>
+  <si>
+    <t>0.694</t>
+  </si>
+  <si>
+    <t>0.820</t>
+  </si>
+  <si>
+    <t>0.722</t>
+  </si>
+  <si>
+    <t>0.798</t>
+  </si>
+  <si>
+    <t>0.567</t>
+  </si>
+  <si>
+    <t>0.651</t>
+  </si>
+  <si>
+    <t>0.936</t>
+  </si>
+  <si>
+    <t>Components:</t>
+  </si>
+  <si>
+    <t>no PCA:</t>
+  </si>
+  <si>
+    <t>PCA, m=8:</t>
+  </si>
+  <si>
+    <t>PCA, m=9:</t>
+  </si>
+  <si>
+    <t>0.754</t>
+  </si>
+  <si>
+    <t>0.711</t>
+  </si>
+  <si>
+    <t>0.769</t>
+  </si>
+  <si>
+    <t>0.423</t>
+  </si>
+  <si>
+    <t>0.579</t>
+  </si>
+  <si>
+    <t>0.838</t>
+  </si>
+  <si>
+    <t>0.341</t>
+  </si>
+  <si>
+    <t>0.538</t>
+  </si>
+  <si>
+    <t>0.667</t>
+  </si>
+  <si>
+    <t>0.839</t>
+  </si>
+  <si>
+    <t>0.663</t>
+  </si>
+  <si>
+    <t>0.639</t>
+  </si>
+  <si>
+    <t>0.417</t>
+  </si>
+  <si>
+    <t>0.460</t>
+  </si>
+  <si>
+    <t>0.522</t>
+  </si>
+  <si>
+    <t>0.483</t>
+  </si>
+  <si>
+    <t>0.582</t>
+  </si>
+  <si>
+    <t>0.337</t>
+  </si>
+  <si>
+    <t>0.501</t>
+  </si>
+  <si>
+    <t>0.657</t>
+  </si>
+  <si>
+    <t>0.644</t>
+  </si>
+  <si>
+    <t>0.750</t>
+  </si>
+  <si>
+    <t>0.859</t>
+  </si>
+  <si>
+    <t>0.424</t>
+  </si>
+  <si>
+    <t>0.493</t>
+  </si>
+  <si>
+    <t>0.551</t>
+  </si>
+  <si>
+    <t>0.822</t>
+  </si>
+  <si>
+    <t>0.728</t>
+  </si>
+  <si>
+    <t>0.801</t>
+  </si>
+  <si>
+    <t>0.439</t>
+  </si>
+  <si>
+    <t>0.524</t>
+  </si>
+  <si>
+    <t>0.629</t>
+  </si>
+  <si>
+    <t>0.675</t>
+  </si>
+  <si>
+    <t>0.710</t>
+  </si>
+  <si>
+    <t>0.760</t>
+  </si>
+  <si>
+    <t>0.823</t>
+  </si>
+  <si>
+    <t>0.771</t>
+  </si>
+  <si>
+    <t>0.431</t>
+  </si>
+  <si>
+    <t>0.432</t>
+  </si>
+  <si>
+    <t>0.426</t>
+  </si>
+  <si>
+    <t>0.469</t>
+  </si>
+  <si>
+    <t>0.499</t>
+  </si>
+  <si>
+    <t>0.443</t>
+  </si>
+  <si>
+    <t>0.504</t>
+  </si>
+  <si>
+    <t>0.515</t>
+  </si>
+  <si>
+    <t>0.523</t>
+  </si>
+  <si>
+    <t>0.573</t>
+  </si>
+  <si>
+    <t>0.478</t>
+  </si>
+  <si>
+    <t>0.467</t>
+  </si>
+  <si>
+    <t>0.577</t>
+  </si>
+  <si>
+    <t>0.816</t>
+  </si>
+  <si>
+    <t>0.511</t>
+  </si>
+  <si>
+    <t>0.520</t>
+  </si>
+  <si>
+    <t>0.507</t>
+  </si>
+  <si>
+    <t>0.525</t>
+  </si>
+  <si>
+    <t>0.770</t>
+  </si>
+  <si>
+    <t>0.875</t>
+  </si>
+  <si>
+    <t>0.891</t>
+  </si>
+  <si>
+    <t>0.768</t>
+  </si>
+  <si>
+    <t>0.451</t>
+  </si>
+  <si>
+    <t>0.506</t>
+  </si>
+  <si>
+    <t>0.521</t>
+  </si>
+  <si>
+    <t>0.516</t>
+  </si>
+  <si>
+    <t>0.554</t>
+  </si>
+  <si>
+    <t>0.668</t>
+  </si>
+  <si>
+    <t>0.780</t>
+  </si>
+  <si>
+    <t>0.975</t>
+  </si>
+  <si>
+    <t>0.509</t>
+  </si>
+  <si>
+    <t>0.527</t>
+  </si>
+  <si>
+    <t>0.530</t>
+  </si>
+  <si>
+    <t>0.532</t>
+  </si>
+  <si>
+    <t>0.678</t>
+  </si>
+  <si>
+    <t>0.456</t>
+  </si>
+  <si>
+    <t>0.555</t>
+  </si>
+  <si>
+    <t>0.570</t>
+  </si>
+  <si>
+    <t>0.547</t>
+  </si>
+  <si>
+    <t>0.753</t>
+  </si>
+  <si>
+    <t>0.775</t>
+  </si>
+  <si>
+    <t>0.955</t>
+  </si>
+  <si>
+    <t>0.989</t>
+  </si>
+  <si>
+    <t>0.529</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -601,7 +884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -609,6 +892,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -925,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C0024B2-0F2E-4A19-B04A-D3E49F7063A9}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1347,7 +1634,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1691,9 +1978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{747763AC-010B-42E1-80AD-99A8E406237E}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1870,4 +2155,706 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F84951-32A8-4D50-B602-1E9362186577}">
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="J3" s="5"/>
+      <c r="L3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>16</v>
+      </c>
+      <c r="H5">
+        <v>32</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>8</v>
+      </c>
+      <c r="P5">
+        <v>16</v>
+      </c>
+      <c r="Q5">
+        <v>32</v>
+      </c>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="K8" t="s">
+        <v>150</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="K9" t="s">
+        <v>151</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="J11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="K12" t="s">
+        <v>150</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="K13" t="s">
+        <v>151</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="K16" t="s">
+        <v>150</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="K17" t="s">
+        <v>151</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="J19" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="K20" t="s">
+        <v>150</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="P20" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q20" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="K21" t="s">
+        <v>151</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q21" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="L3:Q3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cleaning code, adding fusion
</commit_message>
<xml_diff>
--- a/files/results_for_the_report.xlsx
+++ b/files/results_for_the_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krzys\Desktop\ML repo\MLaPR\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1A43C8-61BC-4A0A-8C6B-2A2BC4A7D70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF201C91-B898-4FDA-8EA0-1C156B38898C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8628" yWindow="4236" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="3" xr2:uid="{C99E41AA-753D-4BF4-8020-A2085D88D95B}"/>
+    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{C99E41AA-753D-4BF4-8020-A2085D88D95B}"/>
   </bookViews>
   <sheets>
     <sheet name="MVG Classifiers" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="257">
   <si>
     <t>MVG Classifiers - min DCF</t>
   </si>
@@ -884,6 +884,24 @@
   </si>
   <si>
     <t>error rate: 15.09  %</t>
+  </si>
+  <si>
+    <t>GMM tied full covariance, raw data, PCA (m = 9), components = 2</t>
+  </si>
+  <si>
+    <t>[[885.  97.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [273. 567.]]</t>
+  </si>
+  <si>
+    <t>minDCF: 0.364</t>
+  </si>
+  <si>
+    <t>actDCF: 0.382</t>
+  </si>
+  <si>
+    <t>error rate: 20.31  %</t>
   </si>
 </sst>
 </file>
@@ -977,10 +995,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1319,16 +1337,16 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="G2" s="12" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="G2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -1351,16 +1369,16 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="G5" s="12" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="G5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1467,16 +1485,16 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="G11" s="12" t="s">
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="G11" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1583,16 +1601,16 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="G17" s="12" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="G17" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -1739,16 +1757,16 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="G2" s="12" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="G2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -1771,16 +1789,16 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="G5" s="12" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="G5" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1861,16 +1879,16 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="G10" s="12" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="G10" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
       <c r="L10" t="s">
         <v>123</v>
       </c>
@@ -1954,22 +1972,22 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="G15" s="12" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="G15" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>112</v>
       </c>
       <c r="C16" t="s">
@@ -2083,16 +2101,16 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="G2" s="12" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="G2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -2115,16 +2133,16 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="G5" s="12" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="G5" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2153,16 +2171,16 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="G8" s="12" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="G8" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -2191,16 +2209,16 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="G11" s="12" t="s">
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="G11" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -2248,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F84951-32A8-4D50-B602-1E9362186577}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2268,23 +2286,23 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
       <c r="J3" s="4"/>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
@@ -2948,10 +2966,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72C0C05-0E73-46A1-8F31-E028BDDBDF14}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3049,6 +3067,36 @@
         <v>250</v>
       </c>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>256</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>